<commit_message>
modified script to potentially add other input file types. created a placeholder class for cell, which will later contain all the necessary info to define each of the 81 cell objects
</commit_message>
<xml_diff>
--- a/Sudoku.xlsx
+++ b/Sudoku.xlsx
@@ -159,7 +159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -170,19 +170,16 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -496,16 +493,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="9" width="5.433571428571429" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="4.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="4.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="9" width="4.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="9" width="4.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="9" width="4.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="9" width="4.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="9" width="4.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="9" width="4.005" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="9" width="4.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="8" width="5.433571428571429" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="4.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="8" width="4.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="8" width="4.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="8" width="4.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="8" width="4.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="8" width="4.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="8" width="4.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="8" width="4.005" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="8" width="4.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -546,128 +543,282 @@
         <v>1</v>
       </c>
       <c r="C2" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2" s="3">
-        <v>4</v>
-      </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="E2" s="2">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2">
+        <v>5</v>
+      </c>
+      <c r="G2" s="3">
+        <v>6</v>
+      </c>
+      <c r="H2" s="2">
+        <v>7</v>
+      </c>
+      <c r="I2" s="2">
+        <v>8</v>
+      </c>
+      <c r="J2" s="2">
+        <v>9</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
+      <c r="B3" s="2">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2">
+        <v>5</v>
+      </c>
+      <c r="D3" s="3">
+        <v>6</v>
+      </c>
+      <c r="E3" s="2">
+        <v>7</v>
+      </c>
+      <c r="F3" s="2">
+        <v>8</v>
+      </c>
+      <c r="G3" s="3">
+        <v>9</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1</v>
+      </c>
+      <c r="I3" s="2">
+        <v>2</v>
+      </c>
+      <c r="J3" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
+      <c r="B4" s="4">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4">
+        <v>8</v>
+      </c>
+      <c r="D4" s="5">
+        <v>9</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4">
+        <v>2</v>
+      </c>
+      <c r="G4" s="5">
+        <v>3</v>
+      </c>
+      <c r="H4" s="4">
+        <v>4</v>
+      </c>
+      <c r="I4" s="4">
+        <v>5</v>
+      </c>
+      <c r="J4" s="4">
+        <v>6</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
+      <c r="B5" s="6">
+        <v>2</v>
+      </c>
+      <c r="C5" s="6">
+        <v>3</v>
+      </c>
+      <c r="D5" s="7">
+        <v>4</v>
+      </c>
+      <c r="E5" s="6">
+        <v>5</v>
+      </c>
+      <c r="F5" s="6">
+        <v>6</v>
+      </c>
+      <c r="G5" s="7">
+        <v>7</v>
+      </c>
+      <c r="H5" s="6">
+        <v>8</v>
+      </c>
+      <c r="I5" s="6">
+        <v>9</v>
+      </c>
+      <c r="J5" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
+      <c r="B6" s="2">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2">
+        <v>6</v>
+      </c>
+      <c r="D6" s="3">
+        <v>7</v>
+      </c>
+      <c r="E6" s="2">
+        <v>8</v>
+      </c>
+      <c r="F6" s="2">
+        <v>9</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1</v>
+      </c>
+      <c r="H6" s="2">
+        <v>2</v>
+      </c>
+      <c r="I6" s="2">
+        <v>3</v>
+      </c>
+      <c r="J6" s="2">
+        <v>4</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
+      <c r="B7" s="4">
+        <v>8</v>
+      </c>
+      <c r="C7" s="4">
+        <v>9</v>
+      </c>
+      <c r="D7" s="5">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4">
+        <v>2</v>
+      </c>
+      <c r="F7" s="4">
+        <v>3</v>
+      </c>
+      <c r="G7" s="5">
+        <v>4</v>
+      </c>
+      <c r="H7" s="4">
+        <v>5</v>
+      </c>
+      <c r="I7" s="4">
+        <v>6</v>
+      </c>
+      <c r="J7" s="4">
+        <v>7</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
+      <c r="B8" s="2">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2">
+        <v>4</v>
+      </c>
+      <c r="D8" s="3">
+        <v>5</v>
+      </c>
+      <c r="E8" s="2">
+        <v>6</v>
+      </c>
+      <c r="F8" s="2">
+        <v>7</v>
+      </c>
+      <c r="G8" s="3">
+        <v>8</v>
+      </c>
+      <c r="H8" s="2">
+        <v>9</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0</v>
+      </c>
+      <c r="J8" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
+      <c r="B9" s="2">
+        <v>6</v>
+      </c>
+      <c r="C9" s="2">
+        <v>7</v>
+      </c>
+      <c r="D9" s="3">
+        <v>8</v>
+      </c>
+      <c r="E9" s="2">
+        <v>9</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="3">
+        <v>1</v>
+      </c>
+      <c r="H9" s="2">
+        <v>3</v>
+      </c>
+      <c r="I9" s="2">
+        <v>4</v>
+      </c>
+      <c r="J9" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
+      <c r="B10" s="2">
+        <v>9</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2">
+        <v>3</v>
+      </c>
+      <c r="F10" s="2">
+        <v>4</v>
+      </c>
+      <c r="G10" s="3">
+        <v>5</v>
+      </c>
+      <c r="H10" s="2">
+        <v>6</v>
+      </c>
+      <c r="I10" s="2">
+        <v>7</v>
+      </c>
       <c r="J10" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added functionality that makes an array of cell class objects. The class method identify() lists the location of a given cell and the value it contains (or the value it can be if the value is not set)
</commit_message>
<xml_diff>
--- a/Sudoku.xlsx
+++ b/Sudoku.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>C1</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>C9</t>
+  </si>
+  <si>
+    <t>R0</t>
   </si>
   <si>
     <t>R1</t>
@@ -98,7 +101,14 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -159,30 +169,42 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
   </cellXfs>
@@ -487,51 +509,51 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="8" width="5.433571428571429" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="4.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="8" width="4.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="8" width="4.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="8" width="4.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="8" width="4.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="8" width="4.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="8" width="4.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="8" width="4.005" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="8" width="4.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="10" width="5.433571428571429" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="11" width="4.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="11" width="4.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="11" width="4.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="11" width="4.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="11" width="4.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="11" width="4.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="11" width="4.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="11" width="4.005" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="12" width="4.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1"/>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -539,64 +561,46 @@
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2">
-        <v>2</v>
-      </c>
-      <c r="D2" s="3">
-        <v>3</v>
-      </c>
-      <c r="E2" s="2">
-        <v>4</v>
-      </c>
-      <c r="F2" s="2">
-        <v>5</v>
-      </c>
-      <c r="G2" s="3">
-        <v>6</v>
-      </c>
-      <c r="H2" s="2">
-        <v>7</v>
-      </c>
-      <c r="I2" s="2">
-        <v>8</v>
-      </c>
-      <c r="J2" s="2">
-        <v>9</v>
-      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2">
-        <v>5</v>
-      </c>
-      <c r="D3" s="3">
-        <v>6</v>
-      </c>
-      <c r="E3" s="2">
-        <v>7</v>
-      </c>
-      <c r="F3" s="2">
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4">
+        <v>2</v>
+      </c>
+      <c r="D3" s="5">
+        <v>3</v>
+      </c>
+      <c r="E3" s="4">
+        <v>4</v>
+      </c>
+      <c r="F3" s="4">
+        <v>5</v>
+      </c>
+      <c r="G3" s="5">
+        <v>6</v>
+      </c>
+      <c r="H3" s="4">
+        <v>7</v>
+      </c>
+      <c r="I3" s="4">
         <v>8</v>
       </c>
-      <c r="G3" s="3">
-        <v>9</v>
-      </c>
-      <c r="H3" s="2">
-        <v>1</v>
-      </c>
-      <c r="I3" s="2">
-        <v>2</v>
-      </c>
-      <c r="J3" s="2">
-        <v>3</v>
+      <c r="J3" s="4">
+        <v>9</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
@@ -604,95 +608,95 @@
         <v>11</v>
       </c>
       <c r="B4" s="4">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C4" s="4">
+        <v>5</v>
+      </c>
+      <c r="D4" s="5">
+        <v>6</v>
+      </c>
+      <c r="E4" s="4">
+        <v>7</v>
+      </c>
+      <c r="F4" s="4">
         <v>8</v>
       </c>
-      <c r="D4" s="5">
-        <v>9</v>
-      </c>
-      <c r="E4" s="4">
-        <v>1</v>
-      </c>
-      <c r="F4" s="4">
+      <c r="G4" s="5">
+        <v>9</v>
+      </c>
+      <c r="H4" s="4">
+        <v>1</v>
+      </c>
+      <c r="I4" s="4">
         <v>2</v>
       </c>
-      <c r="G4" s="5">
-        <v>3</v>
-      </c>
-      <c r="H4" s="4">
-        <v>4</v>
-      </c>
-      <c r="I4" s="4">
-        <v>5</v>
-      </c>
       <c r="J4" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+        <v>3</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="6">
+        <v>7</v>
+      </c>
+      <c r="C5" s="6">
+        <v>8</v>
+      </c>
+      <c r="D5" s="7">
+        <v>9</v>
+      </c>
+      <c r="E5" s="6">
+        <v>1</v>
+      </c>
+      <c r="F5" s="6">
         <v>2</v>
       </c>
-      <c r="C5" s="6">
-        <v>3</v>
-      </c>
-      <c r="D5" s="7">
-        <v>4</v>
-      </c>
-      <c r="E5" s="6">
-        <v>5</v>
-      </c>
-      <c r="F5" s="6">
-        <v>6</v>
-      </c>
       <c r="G5" s="7">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H5" s="6">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I5" s="6">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="J5" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+        <v>6</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="2">
-        <v>5</v>
-      </c>
-      <c r="C6" s="2">
-        <v>6</v>
-      </c>
-      <c r="D6" s="3">
-        <v>7</v>
-      </c>
-      <c r="E6" s="2">
+      <c r="B6" s="8">
+        <v>2</v>
+      </c>
+      <c r="C6" s="8">
+        <v>3</v>
+      </c>
+      <c r="D6" s="9">
+        <v>4</v>
+      </c>
+      <c r="E6" s="8">
+        <v>5</v>
+      </c>
+      <c r="F6" s="8">
+        <v>6</v>
+      </c>
+      <c r="G6" s="9">
+        <v>7</v>
+      </c>
+      <c r="H6" s="8">
         <v>8</v>
       </c>
-      <c r="F6" s="2">
-        <v>9</v>
-      </c>
-      <c r="G6" s="3">
-        <v>1</v>
-      </c>
-      <c r="H6" s="2">
-        <v>2</v>
-      </c>
-      <c r="I6" s="2">
-        <v>3</v>
-      </c>
-      <c r="J6" s="2">
-        <v>4</v>
+      <c r="I6" s="8">
+        <v>9</v>
+      </c>
+      <c r="J6" s="8">
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
@@ -700,126 +704,158 @@
         <v>14</v>
       </c>
       <c r="B7" s="4">
+        <v>5</v>
+      </c>
+      <c r="C7" s="4">
+        <v>6</v>
+      </c>
+      <c r="D7" s="5">
+        <v>7</v>
+      </c>
+      <c r="E7" s="4">
         <v>8</v>
       </c>
-      <c r="C7" s="4">
-        <v>9</v>
-      </c>
-      <c r="D7" s="5">
-        <v>1</v>
-      </c>
-      <c r="E7" s="4">
+      <c r="F7" s="4">
+        <v>9</v>
+      </c>
+      <c r="G7" s="5">
+        <v>1</v>
+      </c>
+      <c r="H7" s="4">
         <v>2</v>
       </c>
-      <c r="F7" s="4">
-        <v>3</v>
-      </c>
-      <c r="G7" s="5">
-        <v>4</v>
-      </c>
-      <c r="H7" s="4">
-        <v>5</v>
-      </c>
       <c r="I7" s="4">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="J7" s="4">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+        <v>4</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="2">
-        <v>3</v>
-      </c>
-      <c r="C8" s="2">
-        <v>4</v>
-      </c>
-      <c r="D8" s="3">
-        <v>5</v>
-      </c>
-      <c r="E8" s="2">
-        <v>6</v>
-      </c>
-      <c r="F8" s="2">
-        <v>7</v>
-      </c>
-      <c r="G8" s="3">
+      <c r="B8" s="6">
         <v>8</v>
       </c>
-      <c r="H8" s="2">
-        <v>9</v>
-      </c>
-      <c r="I8" s="2">
-        <v>0</v>
-      </c>
-      <c r="J8" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+      <c r="C8" s="6">
+        <v>9</v>
+      </c>
+      <c r="D8" s="7">
+        <v>1</v>
+      </c>
+      <c r="E8" s="6">
+        <v>2</v>
+      </c>
+      <c r="F8" s="6">
+        <v>3</v>
+      </c>
+      <c r="G8" s="7">
+        <v>4</v>
+      </c>
+      <c r="H8" s="6">
+        <v>5</v>
+      </c>
+      <c r="I8" s="6">
+        <v>6</v>
+      </c>
+      <c r="J8" s="6">
+        <v>7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="2">
-        <v>6</v>
-      </c>
-      <c r="C9" s="2">
-        <v>7</v>
-      </c>
-      <c r="D9" s="3">
+      <c r="B9" s="4">
+        <v>3</v>
+      </c>
+      <c r="C9" s="4">
+        <v>4</v>
+      </c>
+      <c r="D9" s="5">
+        <v>5</v>
+      </c>
+      <c r="E9" s="4">
+        <v>6</v>
+      </c>
+      <c r="F9" s="4">
+        <v>7</v>
+      </c>
+      <c r="G9" s="5">
         <v>8</v>
       </c>
-      <c r="E9" s="2">
-        <v>9</v>
-      </c>
-      <c r="F9" s="2">
+      <c r="H9" s="4">
+        <v>9</v>
+      </c>
+      <c r="I9" s="4">
         <v>0</v>
       </c>
-      <c r="G9" s="3">
-        <v>1</v>
-      </c>
-      <c r="H9" s="2">
-        <v>3</v>
-      </c>
-      <c r="I9" s="2">
-        <v>4</v>
-      </c>
-      <c r="J9" s="2">
-        <v>5</v>
+      <c r="J9" s="4">
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="2">
-        <v>9</v>
-      </c>
-      <c r="C10" s="2">
+      <c r="B10" s="4">
+        <v>6</v>
+      </c>
+      <c r="C10" s="4">
+        <v>7</v>
+      </c>
+      <c r="D10" s="5">
+        <v>8</v>
+      </c>
+      <c r="E10" s="4">
+        <v>9</v>
+      </c>
+      <c r="F10" s="4">
         <v>0</v>
       </c>
-      <c r="D10" s="3">
-        <v>1</v>
-      </c>
-      <c r="E10" s="2">
-        <v>3</v>
-      </c>
-      <c r="F10" s="2">
-        <v>4</v>
-      </c>
-      <c r="G10" s="3">
-        <v>5</v>
-      </c>
-      <c r="H10" s="2">
-        <v>6</v>
-      </c>
-      <c r="I10" s="2">
-        <v>7</v>
-      </c>
-      <c r="J10" s="1"/>
+      <c r="G10" s="5">
+        <v>1</v>
+      </c>
+      <c r="H10" s="4">
+        <v>3</v>
+      </c>
+      <c r="I10" s="4">
+        <v>4</v>
+      </c>
+      <c r="J10" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="4">
+        <v>9</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0</v>
+      </c>
+      <c r="D11" s="5">
+        <v>1</v>
+      </c>
+      <c r="E11" s="4">
+        <v>3</v>
+      </c>
+      <c r="F11" s="4">
+        <v>4</v>
+      </c>
+      <c r="G11" s="5">
+        <v>5</v>
+      </c>
+      <c r="H11" s="4">
+        <v>6</v>
+      </c>
+      <c r="I11" s="4">
+        <v>7</v>
+      </c>
+      <c r="J11" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>